<commit_message>
rename library construction sheet
</commit_message>
<xml_diff>
--- a/templates/dataplant/minSCe/minSCe_-_Single_cell_library_construction.xlsx
+++ b/templates/dataplant/minSCe/minSCe_-_Single_cell_library_construction.xlsx
@@ -9,7 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="isa_template" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="single_cell_library_constructio" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="single_cell_library" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -59,7 +59,7 @@
     <t xml:space="preserve">Table</t>
   </si>
   <si>
-    <t xml:space="preserve">single_cell_library_construction</t>
+    <t xml:space="preserve">single_cell_library</t>
   </si>
   <si>
     <t xml:space="preserve">ERS</t>
@@ -555,10 +555,13 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13:F17"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="42.45"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -654,7 +657,7 @@
       <c r="E13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F13" s="0" t="s">
+      <c r="F13" s="1" t="s">
         <v>23</v>
       </c>
     </row>
@@ -671,7 +674,7 @@
       <c r="D14" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F14" s="0" t="s">
+      <c r="F14" s="1" t="s">
         <v>28</v>
       </c>
     </row>
@@ -688,7 +691,7 @@
       <c r="D15" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F15" s="0" t="s">
+      <c r="F15" s="1" t="s">
         <v>31</v>
       </c>
     </row>
@@ -705,7 +708,7 @@
       <c r="D16" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F16" s="0" t="s">
+      <c r="F16" s="1" t="s">
         <v>36</v>
       </c>
     </row>
@@ -722,7 +725,7 @@
       <c r="D17" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F17" s="0" t="s">
+      <c r="F17" s="1" t="s">
         <v>38</v>
       </c>
     </row>
@@ -840,7 +843,7 @@
   <dimension ref="A1:AJ2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="F13:F17 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>